<commit_message>
Modificato C48 da 10nF a 100nF per possibile instabilità Vref
</commit_message>
<xml_diff>
--- a/ESECUTIVI/LP22-303-0.xlsx
+++ b/ESECUTIVI/LP22-303-0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utenti\00.Lavori in corso\METALTRONICA\22-303-0 (Controllo Collimatore)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\Data\Progetti-GIT\HW\PCB-22-303\ESECUTIVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF72C981-9D51-4B1A-86B1-5513754BF6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE61AEC4-A674-4F26-8C48-17C26970E6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="22-303-0" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="301">
   <si>
     <t>Pos.</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>C1,C7,C8,C9,C11,C15,C16,C17,C19,C23,C24,C25,C27,C31,C32,C33,C35,C39,C40,C41,C43,C45,C46,C49,C50,C51,C52,C53,C54,C58,C63,C69,C71,C72,C73,C74,C75,C77,C78</t>
-  </si>
-  <si>
     <t>MLCC - SMD/SMT 50V 0.1uF X7R 0603 10%</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>SMD1206</t>
   </si>
   <si>
-    <t>C47,C48</t>
-  </si>
-  <si>
     <t>10nF</t>
   </si>
   <si>
@@ -311,21 +305,12 @@
     <t>Fusibili a montaggio superficiale 2 AMP</t>
   </si>
   <si>
-    <t>154 003T</t>
-  </si>
-  <si>
-    <t>150 002T</t>
-  </si>
-  <si>
     <t>LITTELFUSE</t>
   </si>
   <si>
     <t>F6</t>
   </si>
   <si>
-    <t>154 001T</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -518,9 +503,6 @@
     <t>R5,R6</t>
   </si>
   <si>
-    <t>60R</t>
-  </si>
-  <si>
     <t>R8,R17,R26,R35,R44</t>
   </si>
   <si>
@@ -590,9 +572,6 @@
     <t>R58</t>
   </si>
   <si>
-    <t>1K7</t>
-  </si>
-  <si>
     <t>R68,R74,R76,R86</t>
   </si>
   <si>
@@ -861,12 +840,99 @@
   </si>
   <si>
     <t>LISTA PARTI SCHEDA 22-303-0</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB103</t>
+  </si>
+  <si>
+    <t>12063C475KAT4A</t>
+  </si>
+  <si>
+    <t>0154003.DRT</t>
+  </si>
+  <si>
+    <t>0154001.DRT</t>
+  </si>
+  <si>
+    <t>1803277</t>
+  </si>
+  <si>
+    <t>61200621621</t>
+  </si>
+  <si>
+    <t>RC0603FR-1033RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-07120RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-10470RL</t>
+  </si>
+  <si>
+    <t>60R4</t>
+  </si>
+  <si>
+    <t>CRCW060360R4FKEA</t>
+  </si>
+  <si>
+    <t>RC0603FR-07560RL</t>
+  </si>
+  <si>
+    <t>RT0603FRE1324K9L</t>
+  </si>
+  <si>
+    <t>RC0603FR-0715KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-072K2L</t>
+  </si>
+  <si>
+    <t>RC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-071KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-0768RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-1322KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-10820RL</t>
+  </si>
+  <si>
+    <t>1K76</t>
+  </si>
+  <si>
+    <t>RT0603BRD071K76L</t>
+  </si>
+  <si>
+    <t>RC0603FR-13680RL</t>
+  </si>
+  <si>
+    <t>RC1206JR-07330RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-07330RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-07100RL</t>
+  </si>
+  <si>
+    <t>RC1206FR-104K7L</t>
+  </si>
+  <si>
+    <t>C1,C7,C8,C9,C11,C15,C16,C17,C19,C23,C24,C25,C27,C31,C32,C33,C35,C39,C40,C41,C43,C45,C46,C48,C49,C50,C51,C52,C53,C54,C58,C63,C69,C71,C72,C73,C74,C75,C77,C78</t>
+  </si>
+  <si>
+    <t>C47</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1011,7 +1077,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1197,6 +1263,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1373,7 +1445,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1419,6 +1491,18 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1774,11 +1858,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J67"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,11 +1882,11 @@
   <sheetData>
     <row r="1" spans="1:10" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B1" s="14"/>
       <c r="E1" s="13" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F1" s="15"/>
       <c r="I1" s="15"/>
@@ -1844,31 +1928,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="9">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1879,28 +1963,28 @@
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1911,23 +1995,23 @@
         <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="8"/>
     </row>
@@ -1939,20 +2023,20 @@
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="F6" s="10" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="8"/>
@@ -1965,21 +2049,21 @@
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J7" s="8"/>
     </row>
@@ -1988,29 +2072,29 @@
         <v>6</v>
       </c>
       <c r="B8" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>39</v>
+        <v>300</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>41</v>
+        <v>272</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2021,28 +2105,28 @@
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="F9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="H9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2053,28 +2137,28 @@
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="F10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="H10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2085,28 +2169,28 @@
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="F11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="G11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2117,28 +2201,28 @@
         <v>1</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>41</v>
+        <v>273</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2149,28 +2233,28 @@
         <v>2</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="F13" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="H13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="J13" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2181,23 +2265,23 @@
         <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="F14" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>71</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J14" s="8"/>
     </row>
@@ -2209,25 +2293,25 @@
         <v>4</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="G15" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="H15" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J15" s="8"/>
     </row>
@@ -2239,25 +2323,25 @@
         <v>1</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>80</v>
-      </c>
       <c r="H16" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J16" s="8"/>
     </row>
@@ -2269,28 +2353,28 @@
         <v>12</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="F17" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="H17" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="8" t="s">
+      <c r="I17" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="J17" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2301,23 +2385,23 @@
         <v>1</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="F18" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J18" s="8"/>
     </row>
@@ -2329,20 +2413,20 @@
         <v>1</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>95</v>
+        <v>274</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>96</v>
+        <v>274</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="8"/>
@@ -2355,20 +2439,20 @@
         <v>1</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>99</v>
+        <v>275</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>96</v>
+        <v>275</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="8"/>
@@ -2381,58 +2465,58 @@
         <v>1</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D21" s="8" t="s">
+    </row>
+    <row r="22" spans="1:10" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>20</v>
+      </c>
+      <c r="B22" s="17">
+        <v>1</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="D22" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="E22" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="16" t="s">
         <v>102</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>20</v>
-      </c>
-      <c r="B22" s="9">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2443,26 +2527,26 @@
         <v>5</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2473,26 +2557,26 @@
         <v>1</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2503,26 +2587,26 @@
         <v>1</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2533,21 +2617,21 @@
         <v>1</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E26" s="12">
         <v>1803277</v>
       </c>
-      <c r="F26" s="11">
-        <v>1803277</v>
+      <c r="F26" s="11" t="s">
+        <v>276</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J26" s="8"/>
     </row>
@@ -2559,25 +2643,25 @@
         <v>1</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E27" s="12">
         <v>61200621621</v>
       </c>
-      <c r="F27" s="11">
-        <v>61200621621</v>
+      <c r="F27" s="11" t="s">
+        <v>277</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J27" s="8"/>
     </row>
@@ -2589,28 +2673,28 @@
         <v>1</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2621,28 +2705,28 @@
         <v>3</v>
       </c>
       <c r="C29" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="8" t="s">
         <v>133</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2653,28 +2737,28 @@
         <v>1</v>
       </c>
       <c r="C30" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H30" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="I30" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="J30" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2685,11 +2769,11 @@
         <v>5</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="8"/>
@@ -2705,28 +2789,28 @@
         <v>15</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J32" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2737,25 +2821,25 @@
         <v>1</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>41</v>
+        <v>278</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J33" s="8"/>
     </row>
@@ -2767,25 +2851,25 @@
         <v>5</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>41</v>
+        <v>279</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J34" s="8"/>
     </row>
@@ -2797,25 +2881,25 @@
         <v>4</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>41</v>
+        <v>280</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J35" s="8"/>
     </row>
@@ -2827,25 +2911,25 @@
         <v>2</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>164</v>
+        <v>281</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>41</v>
+        <v>282</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J36" s="8"/>
     </row>
@@ -2857,25 +2941,25 @@
         <v>5</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>41</v>
+        <v>283</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J37" s="8"/>
     </row>
@@ -2887,25 +2971,25 @@
         <v>5</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>41</v>
+        <v>284</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J38" s="8"/>
     </row>
@@ -2917,21 +3001,21 @@
         <v>10</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
       <c r="I39" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J39" s="8"/>
     </row>
@@ -2943,25 +3027,25 @@
         <v>6</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>41</v>
+        <v>285</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J40" s="8"/>
     </row>
@@ -2973,25 +3057,25 @@
         <v>7</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>41</v>
+        <v>286</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J41" s="8"/>
     </row>
@@ -3003,25 +3087,25 @@
         <v>11</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>41</v>
+        <v>287</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J42" s="8"/>
     </row>
@@ -3033,25 +3117,25 @@
         <v>6</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>41</v>
+        <v>288</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I43" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J43" s="8"/>
     </row>
@@ -3063,25 +3147,25 @@
         <v>1</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>41</v>
+        <v>289</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J44" s="8"/>
     </row>
@@ -3093,25 +3177,25 @@
         <v>1</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>41</v>
+        <v>290</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I45" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J45" s="8"/>
     </row>
@@ -3123,25 +3207,25 @@
         <v>5</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>41</v>
+        <v>291</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J46" s="8"/>
     </row>
@@ -3153,25 +3237,25 @@
         <v>1</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>188</v>
+        <v>292</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>41</v>
+        <v>293</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I47" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J47" s="8"/>
     </row>
@@ -3183,25 +3267,25 @@
         <v>4</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>41</v>
+        <v>294</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J48" s="8"/>
     </row>
@@ -3213,25 +3297,25 @@
         <v>2</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>41</v>
+        <v>295</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J49" s="8"/>
     </row>
@@ -3243,25 +3327,25 @@
         <v>3</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>41</v>
+        <v>296</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J50" s="8"/>
     </row>
@@ -3273,25 +3357,25 @@
         <v>1</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>41</v>
+        <v>297</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J51" s="8"/>
     </row>
@@ -3303,25 +3387,25 @@
         <v>2</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>41</v>
+        <v>298</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J52" s="8"/>
     </row>
@@ -3333,23 +3417,23 @@
         <v>1</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G53" s="8"/>
       <c r="H53" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="J53" s="8"/>
     </row>
@@ -3361,26 +3445,26 @@
         <v>4</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="G54" s="8"/>
       <c r="H54" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="J54" s="8" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3391,28 +3475,28 @@
         <v>1</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="J55" s="8" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3423,45 +3507,45 @@
         <v>5</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
       <c r="I56" s="10"/>
       <c r="J56" s="8"/>
     </row>
-    <row r="57" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="8">
+    <row r="57" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="16">
         <v>55</v>
       </c>
-      <c r="B57" s="9">
+      <c r="B57" s="17">
         <v>5</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="10"/>
-      <c r="J57" s="8"/>
+      <c r="C57" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="16"/>
     </row>
     <row r="58" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
@@ -3471,16 +3555,16 @@
         <v>5</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
@@ -3495,26 +3579,26 @@
         <v>1</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="8" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J59" s="8" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3525,23 +3609,23 @@
         <v>1</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="G60" s="8"/>
       <c r="H60" s="8" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="J60" s="8"/>
     </row>
@@ -3553,26 +3637,26 @@
         <v>1</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G61" s="8"/>
       <c r="H61" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="J61" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3583,60 +3667,60 @@
         <v>1</v>
       </c>
       <c r="C62" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J62" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="16">
+        <v>61</v>
+      </c>
+      <c r="B63" s="17">
+        <v>1</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="D63" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="E63" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="F63" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G63" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="F62" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="G62" s="8" t="s">
+      <c r="H63" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="I63" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="H62" s="8" t="s">
+      <c r="J63" s="16" t="s">
         <v>242</v>
-      </c>
-      <c r="I62" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="J62" s="8" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="8">
-        <v>61</v>
-      </c>
-      <c r="B63" s="9">
-        <v>1</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="G63" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="H63" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I63" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="J63" s="8" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3647,25 +3731,25 @@
         <v>1</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="J64" s="8"/>
     </row>
@@ -3677,26 +3761,26 @@
         <v>1</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="G65" s="8"/>
       <c r="H65" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="J65" s="8" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3707,25 +3791,25 @@
         <v>2</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="J66" s="8"/>
     </row>
@@ -3737,28 +3821,28 @@
         <v>1</v>
       </c>
       <c r="C67" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="J67" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="F67" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="H67" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="I67" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="J67" s="8" t="s">
-        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3768,7 +3852,7 @@
     <oddFooter>&amp;L&amp;F&amp;C&amp;D&amp;R&amp;Pdi&amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F25 F6 I25" numberStoredAsText="1"/>
+    <ignoredError sqref="I25" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>